<commit_message>
update plots with new risk model a names
</commit_message>
<xml_diff>
--- a/data/pt_characteristics_fine-tuned_models_2024-06-04.xlsx
+++ b/data/pt_characteristics_fine-tuned_models_2024-06-04.xlsx
@@ -521,7 +521,7 @@
         <v>2445</v>
       </c>
       <c r="D4" t="n">
-        <v>1844</v>
+        <v>1797</v>
       </c>
       <c r="E4" t="n">
         <v>201</v>
@@ -541,7 +541,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>19.5 (21.4)</t>
+          <t>19.8 (21.6)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>72 (4.0)</t>
+          <t>72 (4.1)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>628 (34.8)</t>
+          <t>628 (35.8)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>581 (32.2)</t>
+          <t>581 (33.1)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>225 (12.5)</t>
+          <t>225 (12.8)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15 (0.8)</t>
+          <t>15 (0.9)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1259,11 +1259,7 @@
           <t>50 (2.1)</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>47 (2.6)</t>
-        </is>
-      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
@@ -1280,7 +1276,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>194 (10.8)</t>
+          <t>194 (11.0)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>

</xml_diff>